<commit_message>
přidání dat do tabulky
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+  <si>
+    <t xml:space="preserve">i</t>
+  </si>
   <si>
     <t xml:space="preserve">delta T</t>
   </si>
@@ -29,6 +32,18 @@
   </si>
   <si>
     <t xml:space="preserve">měření 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T**2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suma</t>
   </si>
   <si>
     <t xml:space="preserve">E1</t>
@@ -80,9 +95,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -167,7 +183,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -176,7 +192,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -298,10 +322,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.07293121102113"/>
-          <c:y val="0.157843217228159"/>
-          <c:w val="0.883691706227311"/>
-          <c:h val="0.614813606330043"/>
+          <c:x val="0.0729370173969672"/>
+          <c:y val="0.157856093979442"/>
+          <c:w val="0.883663596613638"/>
+          <c:h val="0.614782183064121"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -617,11 +641,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="28654573"/>
-        <c:axId val="75226824"/>
+        <c:axId val="97453052"/>
+        <c:axId val="46672779"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="28654573"/>
+        <c:axId val="97453052"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -653,12 +677,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75226824"/>
+        <c:crossAx val="46672779"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75226824"/>
+        <c:axId val="46672779"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -697,7 +721,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28654573"/>
+        <c:crossAx val="97453052"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -753,16 +777,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>140040</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>25560</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>72000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>35280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>359640</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>426960</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -770,8 +794,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5717880" y="551160"/>
-        <a:ext cx="7734600" cy="4412880"/>
+        <a:off x="9243720" y="736200"/>
+        <a:ext cx="7738920" cy="4412520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -791,11 +815,11 @@
   </sheetPr>
   <dimension ref="B1:I114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G50" activeCellId="0" sqref="G50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.8"/>
@@ -804,185 +828,380 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="1" t="n">
-        <v>100</v>
-      </c>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="1" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="1" t="n">
-        <v>90</v>
-      </c>
-    </row>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="1" t="n">
-        <v>85</v>
+      <c r="B8" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C9" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="2" t="n">
         <v>2.8</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="2" t="n">
         <v>2.8</v>
       </c>
+      <c r="F9" s="3" t="n">
+        <f aca="false">AVERAGE(D9:E9)</f>
+        <v>2.8</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">C9*C9</f>
+        <v>6400</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <f aca="false">F9*C9</f>
+        <v>224</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C10" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="2" t="n">
         <v>2.8</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="2" t="n">
         <v>2.6</v>
       </c>
+      <c r="F10" s="3" t="n">
+        <f aca="false">AVERAGE(D10:E10)</f>
+        <v>2.7</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <f aca="false">C10*C10</f>
+        <v>5625</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <f aca="false">F10*C10</f>
+        <v>202.5</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C11" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="2" t="n">
         <v>2.6</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="2" t="n">
         <v>2.4</v>
       </c>
+      <c r="F11" s="3" t="n">
+        <f aca="false">AVERAGE(D11:E11)</f>
+        <v>2.5</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <f aca="false">C11*C11</f>
+        <v>4900</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <f aca="false">F11*C11</f>
+        <v>175</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C12" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="2" t="n">
         <v>2.4</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="2" t="n">
         <v>2.2</v>
       </c>
+      <c r="F12" s="3" t="n">
+        <f aca="false">AVERAGE(D12:E12)</f>
+        <v>2.3</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <f aca="false">C12*C12</f>
+        <v>4225</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <f aca="false">F12*C12</f>
+        <v>149.5</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C13" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="2" t="n">
         <v>2.2</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="F13" s="3" t="n">
+        <f aca="false">AVERAGE(D13:E13)</f>
+        <v>2.1</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <f aca="false">C13*C13</f>
+        <v>3600</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <f aca="false">F13*C13</f>
+        <v>126</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C14" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="F14" s="3" t="n">
+        <f aca="false">AVERAGE(D14:E14)</f>
+        <v>2</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">C14*C14</f>
+        <v>3025</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">F14*C14</f>
+        <v>110</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C15" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="2" t="n">
         <v>1.8</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="2" t="n">
         <v>1.8</v>
       </c>
+      <c r="F15" s="3" t="n">
+        <f aca="false">AVERAGE(D15:E15)</f>
+        <v>1.8</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <f aca="false">C15*C15</f>
+        <v>2500</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">F15*C15</f>
+        <v>90</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="n">
+        <v>8</v>
+      </c>
       <c r="C16" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="D16" s="2" t="n">
         <v>1.8</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="E16" s="2" t="n">
         <v>1.6</v>
       </c>
+      <c r="F16" s="3" t="n">
+        <f aca="false">AVERAGE(D16:E16)</f>
+        <v>1.7</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <f aca="false">C16*C16</f>
+        <v>2025</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <f aca="false">F16*C16</f>
+        <v>76.5</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="n">
+        <v>9</v>
+      </c>
       <c r="C17" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="D17" s="2" t="n">
         <v>1.6</v>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" s="2" t="n">
         <v>1.4</v>
       </c>
+      <c r="F17" s="3" t="n">
+        <f aca="false">AVERAGE(D17:E17)</f>
+        <v>1.5</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <f aca="false">C17*C17</f>
+        <v>1600</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <f aca="false">F17*C17</f>
+        <v>60</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="n">
+        <v>10</v>
+      </c>
       <c r="C18" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="2" t="n">
         <v>1.2</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="2" t="n">
         <v>1.4</v>
       </c>
+      <c r="F18" s="3" t="n">
+        <f aca="false">AVERAGE(D18:E18)</f>
+        <v>1.3</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <f aca="false">C18*C18</f>
+        <v>1225</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <f aca="false">F18*C18</f>
+        <v>45.5</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="n">
+        <v>11</v>
+      </c>
       <c r="C19" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="2" t="n">
         <v>1.2</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" s="2" t="n">
         <v>1.2</v>
       </c>
+      <c r="F19" s="3" t="n">
+        <f aca="false">AVERAGE(D19:E19)</f>
+        <v>1.2</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <f aca="false">C19*C19</f>
+        <v>900</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <f aca="false">F19*C19</f>
+        <v>36</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="n">
+        <v>12</v>
+      </c>
       <c r="C20" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="D20" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="1" t="n">
+      <c r="E20" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="F20" s="3" t="n">
+        <f aca="false">AVERAGE(D20:E20)</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <f aca="false">C20*C20</f>
+        <v>625</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <f aca="false">F20*C20</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="n">
+        <v>13</v>
+      </c>
       <c r="C21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E21" s="1" t="n">
+      <c r="E21" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <f aca="false">AVERAGE(D21:E21)</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <f aca="false">C21*C21</f>
+        <v>400</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <f aca="false">F21*C21</f>
+        <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1001,25 +1220,37 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <f aca="false">SUM(G9:G21)</f>
+        <v>37050</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <f aca="false">SUM(H9:H21)</f>
+        <v>1340</v>
+      </c>
+    </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="0" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1027,190 +1258,190 @@
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="2" t="n">
+      <c r="C34" s="4" t="n">
         <f aca="false">C9*C9</f>
         <v>6400</v>
       </c>
-      <c r="D34" s="2" t="n">
+      <c r="D34" s="4" t="n">
         <f aca="false">$C9*D9</f>
         <v>224</v>
       </c>
-      <c r="E34" s="2" t="n">
+      <c r="E34" s="4" t="n">
         <f aca="false">$C9*E9</f>
         <v>224</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="2" t="n">
+      <c r="C35" s="4" t="n">
         <f aca="false">C10*C10</f>
         <v>5625</v>
       </c>
-      <c r="D35" s="2" t="n">
+      <c r="D35" s="4" t="n">
         <f aca="false">$C10*D10</f>
         <v>210</v>
       </c>
-      <c r="E35" s="2" t="n">
+      <c r="E35" s="4" t="n">
         <f aca="false">$C10*E10</f>
         <v>195</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="2" t="n">
+      <c r="C36" s="4" t="n">
         <f aca="false">C11*C11</f>
         <v>4900</v>
       </c>
-      <c r="D36" s="2" t="n">
+      <c r="D36" s="4" t="n">
         <f aca="false">$C11*D11</f>
         <v>182</v>
       </c>
-      <c r="E36" s="2" t="n">
+      <c r="E36" s="4" t="n">
         <f aca="false">$C11*E11</f>
         <v>168</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="2" t="n">
+      <c r="C37" s="4" t="n">
         <f aca="false">C12*C12</f>
         <v>4225</v>
       </c>
-      <c r="D37" s="2" t="n">
+      <c r="D37" s="4" t="n">
         <f aca="false">$C12*D12</f>
         <v>156</v>
       </c>
-      <c r="E37" s="2" t="n">
+      <c r="E37" s="4" t="n">
         <f aca="false">$C12*E12</f>
         <v>143</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="2" t="n">
+      <c r="C38" s="4" t="n">
         <f aca="false">C13*C13</f>
         <v>3600</v>
       </c>
-      <c r="D38" s="2" t="n">
+      <c r="D38" s="4" t="n">
         <f aca="false">$C13*D13</f>
         <v>132</v>
       </c>
-      <c r="E38" s="2" t="n">
+      <c r="E38" s="4" t="n">
         <f aca="false">$C13*E13</f>
         <v>120</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="2" t="n">
+      <c r="C39" s="4" t="n">
         <f aca="false">C14*C14</f>
         <v>3025</v>
       </c>
-      <c r="D39" s="2" t="n">
+      <c r="D39" s="4" t="n">
         <f aca="false">$C14*D14</f>
         <v>110</v>
       </c>
-      <c r="E39" s="2" t="n">
+      <c r="E39" s="4" t="n">
         <f aca="false">$C14*E14</f>
         <v>110</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="2" t="n">
+      <c r="C40" s="4" t="n">
         <f aca="false">C15*C15</f>
         <v>2500</v>
       </c>
-      <c r="D40" s="2" t="n">
+      <c r="D40" s="4" t="n">
         <f aca="false">$C15*D15</f>
         <v>90</v>
       </c>
-      <c r="E40" s="2" t="n">
+      <c r="E40" s="4" t="n">
         <f aca="false">$C15*E15</f>
         <v>90</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="2" t="n">
+      <c r="C41" s="4" t="n">
         <f aca="false">C16*C16</f>
         <v>2025</v>
       </c>
-      <c r="D41" s="2" t="n">
+      <c r="D41" s="4" t="n">
         <f aca="false">$C16*D16</f>
         <v>81</v>
       </c>
-      <c r="E41" s="2" t="n">
+      <c r="E41" s="4" t="n">
         <f aca="false">$C16*E16</f>
         <v>72</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="2" t="n">
+      <c r="C42" s="4" t="n">
         <f aca="false">C17*C17</f>
         <v>1600</v>
       </c>
-      <c r="D42" s="2" t="n">
+      <c r="D42" s="4" t="n">
         <f aca="false">$C17*D17</f>
         <v>64</v>
       </c>
-      <c r="E42" s="2" t="n">
+      <c r="E42" s="4" t="n">
         <f aca="false">$C17*E17</f>
         <v>56</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="2" t="n">
+      <c r="C43" s="4" t="n">
         <f aca="false">C18*C18</f>
         <v>1225</v>
       </c>
-      <c r="D43" s="2" t="n">
+      <c r="D43" s="4" t="n">
         <f aca="false">$C18*D18</f>
         <v>42</v>
       </c>
-      <c r="E43" s="2" t="n">
+      <c r="E43" s="4" t="n">
         <f aca="false">$C18*E18</f>
         <v>49</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="2" t="n">
+      <c r="C44" s="4" t="n">
         <f aca="false">C19*C19</f>
         <v>900</v>
       </c>
-      <c r="D44" s="2" t="n">
+      <c r="D44" s="4" t="n">
         <f aca="false">$C19*D19</f>
         <v>36</v>
       </c>
-      <c r="E44" s="2" t="n">
+      <c r="E44" s="4" t="n">
         <f aca="false">$C19*E19</f>
         <v>36</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="2" t="n">
+      <c r="C45" s="4" t="n">
         <f aca="false">C20*C20</f>
         <v>625</v>
       </c>
-      <c r="D45" s="2" t="n">
+      <c r="D45" s="4" t="n">
         <f aca="false">$C20*D20</f>
         <v>25</v>
       </c>
-      <c r="E45" s="2" t="n">
+      <c r="E45" s="4" t="n">
         <f aca="false">$C20*E20</f>
         <v>25</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="2" t="n">
+      <c r="C46" s="4" t="n">
         <f aca="false">C21*C21</f>
         <v>400</v>
       </c>
-      <c r="D46" s="2" t="n">
+      <c r="D46" s="4" t="n">
         <f aca="false">$C21*D21</f>
         <v>20</v>
       </c>
-      <c r="E46" s="2" t="n">
+      <c r="E46" s="4" t="n">
         <f aca="false">$C21*E21</f>
         <v>20</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C48" s="0" t="n">
         <f aca="false">SUM(C34:C46)</f>
@@ -1227,7 +1458,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D50" s="0" t="n">
         <f aca="false">D48/$C48</f>
@@ -1309,19 +1540,19 @@
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,7 +2077,7 @@
     </row>
     <row r="108" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C108" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D108" s="0" t="n">
         <f aca="false">AVERAGE(D80:D105)</f>
@@ -1855,7 +2086,7 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C109" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F109" s="0" t="n">
         <f aca="false">SUM(F80:F105)</f>
@@ -1869,7 +2100,7 @@
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D112" s="0" t="n">
         <f aca="false">1-F109/G109</f>
@@ -1878,7 +2109,7 @@
     </row>
     <row r="114" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C114" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D114" s="0" t="n">
         <f aca="false">SQRT(D112)</f>

</xml_diff>